<commit_message>
complete the course registration
</commit_message>
<xml_diff>
--- a/Work Plan and Task Breakdown.xlsx
+++ b/Work Plan and Task Breakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CureUniversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6AB24F-7517-4011-9497-47DBE0E63F16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D540F2-A74E-4659-B00C-8243EACCC84C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{CA06B390-A52D-437A-980B-D056BC637CE4}"/>
   </bookViews>
@@ -305,7 +305,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +330,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -343,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -367,6 +373,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D939D964-A973-405E-8CB0-E30FD15B986D}">
   <dimension ref="A1:R195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1076,7 +1087,7 @@
         <v>43872</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>2</v>
       </c>
@@ -1087,20 +1098,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>27</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="N34" s="17"/>
+      <c r="O34" s="12">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>50</v>
       </c>
@@ -1111,7 +1126,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
         <v>25</v>
       </c>
@@ -1119,12 +1134,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>8</v>
       </c>
@@ -1135,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>9</v>
       </c>
@@ -1143,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>10</v>
       </c>
@@ -1151,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
@@ -1160,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6" t="s">
@@ -1173,7 +1188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6" t="s">
@@ -1184,12 +1199,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>30</v>
       </c>
@@ -1197,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
         <v>2</v>
       </c>
@@ -1208,7 +1223,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>31</v>
       </c>
@@ -1216,12 +1231,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>50</v>
       </c>
@@ -1236,7 +1251,7 @@
         <v>16.75</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>47</v>
       </c>
@@ -1244,12 +1259,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
         <v>8</v>
       </c>
@@ -1260,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
         <v>18</v>
       </c>
@@ -1268,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>10</v>
       </c>
@@ -1276,12 +1291,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E56">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>12</v>
       </c>
@@ -1292,7 +1307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
         <v>33</v>
       </c>
@@ -1303,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>34</v>
       </c>
@@ -1311,116 +1326,151 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E60">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="1" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="15"/>
+      <c r="B61" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="15"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="15"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="15"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C67" t="s">
+      <c r="D65" s="17"/>
+      <c r="E65" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="15"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="15"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="17">
         <v>0.75</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C68" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="15"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C69" t="s">
+      <c r="D68" s="17"/>
+      <c r="E68" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="15"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C71" t="s">
+      <c r="D69" s="17"/>
+      <c r="E69" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="15"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="15"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="17">
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C72" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="15"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D72" s="17"/>
+      <c r="E72" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B74" s="1" t="s">
         <v>38</v>
       </c>
@@ -1428,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
         <v>2</v>
       </c>
@@ -1439,7 +1489,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
         <v>42</v>
       </c>
@@ -1447,12 +1497,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E77">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
         <v>39</v>
       </c>
@@ -1460,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
         <v>40</v>
       </c>
@@ -1472,7 +1522,7 @@
         <v>22.75</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E80">
         <v>0</v>
       </c>

</xml_diff>